<commit_message>
Update test report data for registerTest and adjust statistics
- Changed test suite output to reflect new test case 'registerTest'.
- Updated strings to include relevant information for 'registerTest'.
- Modified statistics to indicate successful execution of 'registerTest' with no failures.
- Adjusted timestamps and generated report metrics accordingly.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/AddShift.xlsx
+++ b/ProjectTest65/Excel/AddShift.xlsx
@@ -489,8 +489,8 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="84" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -733,7 +733,7 @@
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B5" s="4" t="n">
@@ -782,7 +782,7 @@
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B6" s="4" t="n">
@@ -994,7 +994,7 @@
     <row r="10" ht="18.75" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B10" s="4" t="n">
@@ -1414,7 +1414,7 @@
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B18" s="4" t="n">
@@ -1873,7 +1873,11 @@
           <t>ความยาวตัวอักษรตั้งแต่ 6 – 50 ตัวอักษร</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>เกิดข้อผิดพลาด กรุณาลองใหม่อีกครั้ง !!!</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>Fail</t>
@@ -1883,7 +1887,7 @@
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B27" s="4" t="n">
@@ -1918,9 +1922,14 @@
           <t>กรุณากรอกการรับหน้าที่</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>กรุณากรอกการรับหน้าที่</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update report.html with new test results and metadata
- Changed suite data to reflect updated test execution results.
- Updated strings to include new test case for registration.
- Modified stats to show elapsed time and results for the registerTest.
- Adjusted baseMillis and generated values to match the latest test run.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/AddShift.xlsx
+++ b/ProjectTest65/Excel/AddShift.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6375" yWindow="2985" windowWidth="12585" windowHeight="11235" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddShift" sheetId="1" state="visible" r:id="rId1"/>
@@ -489,24 +489,24 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="L5" sqref="J5:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="24.109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="11.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="9.5546875" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.88671875" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="40.33203125" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="37.5546875" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="35.44140625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="20.88671875" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="24.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="9.5703125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.85546875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="40.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="37.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="35.42578125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="20.85546875" bestFit="1" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -782,7 +782,7 @@
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B6" s="4" t="n">
@@ -994,7 +994,7 @@
     <row r="10" ht="18.75" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B10" s="4" t="n">
@@ -1414,7 +1414,7 @@
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B18" s="4" t="n">
@@ -1834,7 +1834,7 @@
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B26" s="4" t="n">
@@ -1887,7 +1887,7 @@
     <row r="27" ht="18.75" customHeight="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B27" s="4" t="n">

</xml_diff>